<commit_message>
add random reschedule function
</commit_message>
<xml_diff>
--- a/f_iden_3.xlsx
+++ b/f_iden_3.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PC\Share\Programing\SAMURAI\Students\2023\Corp_2311_Ricoh\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PC\Share\Programing\SAMURAI\Students\2023\Corp_2311_Ricoh\AutoScheduler\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="900" windowWidth="28800" windowHeight="12585"/>
+    <workbookView xWindow="0" yWindow="450" windowWidth="7470" windowHeight="8280" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="koutei" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="73">
   <si>
     <t>ジャストインタイム</t>
   </si>
@@ -241,6 +241,9 @@
   <si>
     <t>※赤字：未</t>
   </si>
+  <si>
+    <t>製造番号</t>
+  </si>
 </sst>
 </file>
 
@@ -249,7 +252,7 @@
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="m/d"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -287,6 +290,13 @@
       <name val="ＭＳ Ｐゴシック"/>
       <family val="3"/>
       <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -343,10 +353,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -407,9 +418,12 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="3" fontId="6" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
+    <cellStyle name="標準 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -714,7 +728,7 @@
   </sheetPr>
   <dimension ref="A1:R30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
@@ -2194,144 +2208,148 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:AH53"/>
+  <dimension ref="A1:AI53"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E56" sqref="E56"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="16.625" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.625" style="13" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.875" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.625" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="14" width="13.625" style="6" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.125" style="6" bestFit="1" customWidth="1"/>
-    <col min="16" max="33" width="13.625" style="6" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="13.625" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.625" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.625" style="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.875" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.625" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="15" width="13.625" style="6" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.125" style="6" bestFit="1" customWidth="1"/>
+    <col min="17" max="34" width="13.625" style="6" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="13.625" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:35" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="24" t="s">
+        <v>72</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="C1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="D1" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="9">
+      <c r="E1" s="9">
         <v>45078</v>
       </c>
-      <c r="E1" s="9">
+      <c r="F1" s="9">
         <v>45079</v>
       </c>
-      <c r="F1" s="5">
+      <c r="G1" s="5">
         <v>45080</v>
       </c>
-      <c r="G1" s="5">
+      <c r="H1" s="5">
         <v>45081</v>
       </c>
-      <c r="H1" s="9">
+      <c r="I1" s="9">
         <v>45082</v>
       </c>
-      <c r="I1" s="9">
+      <c r="J1" s="9">
         <v>45083</v>
       </c>
-      <c r="J1" s="9">
+      <c r="K1" s="9">
         <v>45084</v>
       </c>
-      <c r="K1" s="9">
+      <c r="L1" s="9">
         <v>45085</v>
       </c>
-      <c r="L1" s="9">
+      <c r="M1" s="9">
         <v>45086</v>
       </c>
-      <c r="M1" s="5">
+      <c r="N1" s="5">
         <v>45087</v>
       </c>
-      <c r="N1" s="5">
+      <c r="O1" s="5">
         <v>45088</v>
       </c>
-      <c r="O1" s="9">
+      <c r="P1" s="9">
         <v>45089</v>
       </c>
-      <c r="P1" s="9">
+      <c r="Q1" s="9">
         <v>45090</v>
       </c>
-      <c r="Q1" s="9">
+      <c r="R1" s="9">
         <v>45091</v>
       </c>
-      <c r="R1" s="9">
+      <c r="S1" s="9">
         <v>45092</v>
       </c>
-      <c r="S1" s="9">
+      <c r="T1" s="9">
         <v>45093</v>
       </c>
-      <c r="T1" s="5">
+      <c r="U1" s="5">
         <v>45094</v>
       </c>
-      <c r="U1" s="5">
+      <c r="V1" s="5">
         <v>45095</v>
       </c>
-      <c r="V1" s="9">
+      <c r="W1" s="9">
         <v>45096</v>
       </c>
-      <c r="W1" s="9">
+      <c r="X1" s="9">
         <v>45097</v>
       </c>
-      <c r="X1" s="9">
+      <c r="Y1" s="9">
         <v>45098</v>
       </c>
-      <c r="Y1" s="9">
+      <c r="Z1" s="9">
         <v>45099</v>
       </c>
-      <c r="Z1" s="9">
+      <c r="AA1" s="9">
         <v>45100</v>
       </c>
-      <c r="AA1" s="5">
+      <c r="AB1" s="5">
         <v>45101</v>
       </c>
-      <c r="AB1" s="5">
+      <c r="AC1" s="5">
         <v>45102</v>
       </c>
-      <c r="AC1" s="9">
+      <c r="AD1" s="9">
         <v>45103</v>
       </c>
-      <c r="AD1" s="9">
+      <c r="AE1" s="9">
         <v>45104</v>
       </c>
-      <c r="AE1" s="9">
+      <c r="AF1" s="9">
         <v>45105</v>
       </c>
-      <c r="AF1" s="9">
+      <c r="AG1" s="9">
         <v>45106</v>
       </c>
-      <c r="AG1" s="9">
+      <c r="AH1" s="9">
         <v>45107</v>
       </c>
-      <c r="AH1" s="2"/>
-    </row>
-    <row r="2" spans="1:34" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="10" t="s">
+      <c r="AI1" s="2"/>
+    </row>
+    <row r="2" spans="1:35" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="25">
+        <v>1</v>
+      </c>
+      <c r="B2" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="11">
+      <c r="C2" s="11">
         <v>1</v>
       </c>
-      <c r="C2" s="5">
+      <c r="D2" s="5">
         <v>45089</v>
       </c>
-      <c r="D2" s="12" t="str">
-        <f>IF($C2=D$1,"☆","")</f>
-        <v/>
-      </c>
       <c r="E2" s="12" t="str">
-        <f t="shared" ref="E2:AH10" si="0">IF($C2=E$1,"☆","")</f>
+        <f>IF($D2=E$1,"☆","")</f>
         <v/>
       </c>
       <c r="F2" s="12" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="F2:AI10" si="0">IF($D2=F$1,"☆","")</f>
         <v/>
       </c>
       <c r="G2" s="12" t="str">
@@ -2368,12 +2386,12 @@
       </c>
       <c r="O2" s="12" t="str">
         <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="P2" s="12" t="str">
+        <f t="shared" si="0"/>
         <v>☆</v>
       </c>
-      <c r="P2" s="12" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
       <c r="Q2" s="12" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2446,23 +2464,26 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-    </row>
-    <row r="3" spans="1:34" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="10" t="s">
+      <c r="AI2" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="3" spans="1:35" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="25">
+        <v>1</v>
+      </c>
+      <c r="B3" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="11">
+      <c r="C3" s="11">
         <v>2</v>
       </c>
-      <c r="C3" s="5">
+      <c r="D3" s="5">
         <v>45089</v>
       </c>
-      <c r="D3" s="12" t="str">
-        <f t="shared" ref="D3:S34" si="1">IF($C3=D$1,"☆","")</f>
-        <v/>
-      </c>
       <c r="E3" s="12" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="E3:T26" si="1">IF($D3=E$1,"☆","")</f>
         <v/>
       </c>
       <c r="F3" s="12" t="str">
@@ -2503,12 +2524,12 @@
       </c>
       <c r="O3" s="12" t="str">
         <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="P3" s="12" t="str">
+        <f t="shared" si="0"/>
         <v>☆</v>
       </c>
-      <c r="P3" s="12" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
       <c r="Q3" s="12" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2581,23 +2602,26 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-    </row>
-    <row r="4" spans="1:34" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="10" t="s">
+      <c r="AI3" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="4" spans="1:35" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="25">
+        <v>1</v>
+      </c>
+      <c r="B4" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="11">
+      <c r="C4" s="11">
         <v>3</v>
       </c>
-      <c r="C4" s="5">
+      <c r="D4" s="5">
         <v>45089</v>
       </c>
-      <c r="D4" s="12" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
       <c r="E4" s="12" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="F4" s="12" t="str">
@@ -2638,12 +2662,12 @@
       </c>
       <c r="O4" s="12" t="str">
         <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="P4" s="12" t="str">
+        <f t="shared" si="0"/>
         <v>☆</v>
       </c>
-      <c r="P4" s="12" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
       <c r="Q4" s="12" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2716,23 +2740,26 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-    </row>
-    <row r="5" spans="1:34" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="10" t="s">
+      <c r="AI4" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="5" spans="1:35" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="25">
+        <v>2</v>
+      </c>
+      <c r="B5" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="11">
+      <c r="C5" s="11">
         <v>1</v>
       </c>
-      <c r="C5" s="5">
+      <c r="D5" s="5">
         <v>45099</v>
       </c>
-      <c r="D5" s="12" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
       <c r="E5" s="12" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="F5" s="12" t="str">
@@ -2813,12 +2840,12 @@
       </c>
       <c r="Y5" s="12" t="str">
         <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="Z5" s="12" t="str">
+        <f t="shared" si="0"/>
         <v>☆</v>
       </c>
-      <c r="Z5" s="12" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
       <c r="AA5" s="12" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2851,23 +2878,26 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-    </row>
-    <row r="6" spans="1:34" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="10" t="s">
+      <c r="AI5" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="6" spans="1:35" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="25">
+        <v>2</v>
+      </c>
+      <c r="B6" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="11">
+      <c r="C6" s="11">
         <v>2</v>
       </c>
-      <c r="C6" s="5">
+      <c r="D6" s="5">
         <v>45099</v>
       </c>
-      <c r="D6" s="12" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
       <c r="E6" s="12" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="F6" s="12" t="str">
@@ -2948,12 +2978,12 @@
       </c>
       <c r="Y6" s="12" t="str">
         <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="Z6" s="12" t="str">
+        <f t="shared" si="0"/>
         <v>☆</v>
       </c>
-      <c r="Z6" s="12" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
       <c r="AA6" s="12" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2986,23 +3016,26 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-    </row>
-    <row r="7" spans="1:34" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="10" t="s">
+      <c r="AI6" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="7" spans="1:35" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="25">
+        <v>2</v>
+      </c>
+      <c r="B7" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="11">
+      <c r="C7" s="11">
         <v>3</v>
       </c>
-      <c r="C7" s="5">
+      <c r="D7" s="5">
         <v>45099</v>
       </c>
-      <c r="D7" s="12" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
       <c r="E7" s="12" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="F7" s="12" t="str">
@@ -3083,12 +3116,12 @@
       </c>
       <c r="Y7" s="12" t="str">
         <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="Z7" s="12" t="str">
+        <f t="shared" si="0"/>
         <v>☆</v>
       </c>
-      <c r="Z7" s="12" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
       <c r="AA7" s="12" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -3121,23 +3154,26 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-    </row>
-    <row r="8" spans="1:34" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="10" t="s">
+      <c r="AI7" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="8" spans="1:35" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="25">
+        <v>2</v>
+      </c>
+      <c r="B8" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="11">
+      <c r="C8" s="11">
         <v>4</v>
       </c>
-      <c r="C8" s="5">
+      <c r="D8" s="5">
         <v>45099</v>
       </c>
-      <c r="D8" s="12" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
       <c r="E8" s="12" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="F8" s="12" t="str">
@@ -3218,12 +3254,12 @@
       </c>
       <c r="Y8" s="12" t="str">
         <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="Z8" s="12" t="str">
+        <f t="shared" si="0"/>
         <v>☆</v>
       </c>
-      <c r="Z8" s="12" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
       <c r="AA8" s="12" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -3256,23 +3292,26 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-    </row>
-    <row r="9" spans="1:34" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="10" t="s">
+      <c r="AI8" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="9" spans="1:35" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="25">
+        <v>3</v>
+      </c>
+      <c r="B9" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="11">
+      <c r="C9" s="11">
         <v>1</v>
       </c>
-      <c r="C9" s="5">
+      <c r="D9" s="5">
         <v>45107</v>
       </c>
-      <c r="D9" s="12" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
       <c r="E9" s="12" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="F9" s="12" t="str">
@@ -3385,29 +3424,32 @@
       </c>
       <c r="AG9" s="12" t="str">
         <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AH9" s="12" t="str">
+        <f t="shared" si="0"/>
         <v>☆</v>
       </c>
-      <c r="AH9" s="12" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="10" spans="1:34" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="10" t="s">
+      <c r="AI9" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="10" spans="1:35" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="25">
+        <v>4</v>
+      </c>
+      <c r="B10" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="11">
+      <c r="C10" s="11">
         <v>1</v>
       </c>
-      <c r="C10" s="5">
+      <c r="D10" s="5">
         <v>45103</v>
       </c>
-      <c r="D10" s="12" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
       <c r="E10" s="12" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="F10" s="12" t="str">
@@ -3467,11 +3509,11 @@
         <v/>
       </c>
       <c r="T10" s="12" t="str">
-        <f t="shared" ref="T10:AH53" si="2">IF($C10=T$1,"☆","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="U10" s="12" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="U10:AI27" si="2">IF($D10=U$1,"☆","")</f>
         <v/>
       </c>
       <c r="V10" s="12" t="str">
@@ -3504,12 +3546,12 @@
       </c>
       <c r="AC10" s="12" t="str">
         <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="AD10" s="12" t="str">
+        <f t="shared" si="2"/>
         <v>☆</v>
       </c>
-      <c r="AD10" s="12" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
       <c r="AE10" s="12" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -3526,21 +3568,24 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-    </row>
-    <row r="11" spans="1:34" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="10" t="s">
+      <c r="AI10" s="12" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="11" spans="1:35" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A11" s="25">
+        <v>4</v>
+      </c>
+      <c r="B11" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="11">
+      <c r="C11" s="11">
         <v>2</v>
       </c>
-      <c r="C11" s="5">
+      <c r="D11" s="5">
         <v>45103</v>
       </c>
-      <c r="D11" s="12" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
       <c r="E11" s="12" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -3602,7 +3647,7 @@
         <v/>
       </c>
       <c r="T11" s="12" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="U11" s="12" t="str">
@@ -3639,12 +3684,12 @@
       </c>
       <c r="AC11" s="12" t="str">
         <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="AD11" s="12" t="str">
+        <f t="shared" si="2"/>
         <v>☆</v>
       </c>
-      <c r="AD11" s="12" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
       <c r="AE11" s="12" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -3661,21 +3706,24 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-    </row>
-    <row r="12" spans="1:34" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="10" t="s">
+      <c r="AI11" s="12" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="12" spans="1:35" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A12" s="25">
+        <v>5</v>
+      </c>
+      <c r="B12" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="11">
+      <c r="C12" s="11">
         <v>1</v>
       </c>
-      <c r="C12" s="5">
+      <c r="D12" s="5">
         <v>45099</v>
       </c>
-      <c r="D12" s="12" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
       <c r="E12" s="12" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -3737,7 +3785,7 @@
         <v/>
       </c>
       <c r="T12" s="12" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="U12" s="12" t="str">
@@ -3758,12 +3806,12 @@
       </c>
       <c r="Y12" s="12" t="str">
         <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="Z12" s="12" t="str">
+        <f t="shared" si="2"/>
         <v>☆</v>
       </c>
-      <c r="Z12" s="12" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
       <c r="AA12" s="12" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -3796,21 +3844,24 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-    </row>
-    <row r="13" spans="1:34" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="10" t="s">
+      <c r="AI12" s="12" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="13" spans="1:35" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="25">
+        <v>5</v>
+      </c>
+      <c r="B13" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="11">
+      <c r="C13" s="11">
         <v>2</v>
       </c>
-      <c r="C13" s="5">
+      <c r="D13" s="5">
         <v>45099</v>
       </c>
-      <c r="D13" s="12" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
       <c r="E13" s="12" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -3872,7 +3923,7 @@
         <v/>
       </c>
       <c r="T13" s="12" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="U13" s="12" t="str">
@@ -3893,12 +3944,12 @@
       </c>
       <c r="Y13" s="12" t="str">
         <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="Z13" s="12" t="str">
+        <f t="shared" si="2"/>
         <v>☆</v>
       </c>
-      <c r="Z13" s="12" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
       <c r="AA13" s="12" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -3931,21 +3982,24 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-    </row>
-    <row r="14" spans="1:34" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="10" t="s">
+      <c r="AI13" s="12" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="14" spans="1:35" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A14" s="25">
+        <v>5</v>
+      </c>
+      <c r="B14" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="11">
+      <c r="C14" s="11">
         <v>3</v>
       </c>
-      <c r="C14" s="5">
+      <c r="D14" s="5">
         <v>45099</v>
       </c>
-      <c r="D14" s="12" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
       <c r="E14" s="12" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -4007,7 +4061,7 @@
         <v/>
       </c>
       <c r="T14" s="12" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="U14" s="12" t="str">
@@ -4028,12 +4082,12 @@
       </c>
       <c r="Y14" s="12" t="str">
         <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="Z14" s="12" t="str">
+        <f t="shared" si="2"/>
         <v>☆</v>
       </c>
-      <c r="Z14" s="12" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
       <c r="AA14" s="12" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -4066,21 +4120,24 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-    </row>
-    <row r="15" spans="1:34" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A15" s="10" t="s">
+      <c r="AI14" s="12" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="15" spans="1:35" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A15" s="25">
+        <v>5</v>
+      </c>
+      <c r="B15" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B15" s="11">
+      <c r="C15" s="11">
         <v>4</v>
       </c>
-      <c r="C15" s="5">
+      <c r="D15" s="5">
         <v>45099</v>
       </c>
-      <c r="D15" s="12" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
       <c r="E15" s="12" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -4142,7 +4199,7 @@
         <v/>
       </c>
       <c r="T15" s="12" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="U15" s="12" t="str">
@@ -4163,12 +4220,12 @@
       </c>
       <c r="Y15" s="12" t="str">
         <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="Z15" s="12" t="str">
+        <f t="shared" si="2"/>
         <v>☆</v>
       </c>
-      <c r="Z15" s="12" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
       <c r="AA15" s="12" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -4201,21 +4258,24 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-    </row>
-    <row r="16" spans="1:34" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="10" t="s">
+      <c r="AI15" s="12" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="16" spans="1:35" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A16" s="25">
+        <v>6</v>
+      </c>
+      <c r="B16" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="B16" s="11">
+      <c r="C16" s="11">
         <v>1</v>
       </c>
-      <c r="C16" s="5">
+      <c r="D16" s="5">
         <v>45096</v>
       </c>
-      <c r="D16" s="12" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
       <c r="E16" s="12" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -4277,7 +4337,7 @@
         <v/>
       </c>
       <c r="T16" s="12" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="U16" s="12" t="str">
@@ -4286,12 +4346,12 @@
       </c>
       <c r="V16" s="12" t="str">
         <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="W16" s="12" t="str">
+        <f t="shared" si="2"/>
         <v>☆</v>
       </c>
-      <c r="W16" s="12" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
       <c r="X16" s="12" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -4336,21 +4396,24 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-    </row>
-    <row r="17" spans="1:34" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="10" t="s">
+      <c r="AI16" s="12" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="17" spans="1:35" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A17" s="25">
+        <v>7</v>
+      </c>
+      <c r="B17" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="B17" s="11">
+      <c r="C17" s="11">
         <v>1</v>
       </c>
-      <c r="C17" s="5">
+      <c r="D17" s="5">
         <v>45097</v>
       </c>
-      <c r="D17" s="12" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
       <c r="E17" s="12" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -4412,7 +4475,7 @@
         <v/>
       </c>
       <c r="T17" s="12" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="U17" s="12" t="str">
@@ -4425,12 +4488,12 @@
       </c>
       <c r="W17" s="12" t="str">
         <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="X17" s="12" t="str">
+        <f t="shared" si="2"/>
         <v>☆</v>
       </c>
-      <c r="X17" s="12" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
       <c r="Y17" s="12" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -4471,21 +4534,24 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-    </row>
-    <row r="18" spans="1:34" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A18" s="10" t="s">
+      <c r="AI17" s="12" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="18" spans="1:35" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A18" s="25">
+        <v>8</v>
+      </c>
+      <c r="B18" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="B18" s="11">
+      <c r="C18" s="11">
         <v>1</v>
       </c>
-      <c r="C18" s="5">
+      <c r="D18" s="5">
         <v>45098</v>
       </c>
-      <c r="D18" s="12" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
       <c r="E18" s="12" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -4547,7 +4613,7 @@
         <v/>
       </c>
       <c r="T18" s="12" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="U18" s="12" t="str">
@@ -4564,12 +4630,12 @@
       </c>
       <c r="X18" s="12" t="str">
         <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="Y18" s="12" t="str">
+        <f t="shared" si="2"/>
         <v>☆</v>
       </c>
-      <c r="Y18" s="12" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
       <c r="Z18" s="12" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -4606,21 +4672,24 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-    </row>
-    <row r="19" spans="1:34" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="10" t="s">
+      <c r="AI18" s="12" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="19" spans="1:35" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A19" s="25">
+        <v>6</v>
+      </c>
+      <c r="B19" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="B19" s="11">
+      <c r="C19" s="11">
         <v>2</v>
       </c>
-      <c r="C19" s="5">
+      <c r="D19" s="5">
         <v>45096</v>
       </c>
-      <c r="D19" s="12" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
       <c r="E19" s="12" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -4682,7 +4751,7 @@
         <v/>
       </c>
       <c r="T19" s="12" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="U19" s="12" t="str">
@@ -4691,12 +4760,12 @@
       </c>
       <c r="V19" s="12" t="str">
         <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="W19" s="12" t="str">
+        <f t="shared" si="2"/>
         <v>☆</v>
       </c>
-      <c r="W19" s="12" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
       <c r="X19" s="12" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -4741,21 +4810,24 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-    </row>
-    <row r="20" spans="1:34" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="10" t="s">
+      <c r="AI19" s="12" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="20" spans="1:35" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A20" s="25">
+        <v>7</v>
+      </c>
+      <c r="B20" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="B20" s="11">
+      <c r="C20" s="11">
         <v>2</v>
       </c>
-      <c r="C20" s="5">
+      <c r="D20" s="5">
         <v>45097</v>
       </c>
-      <c r="D20" s="12" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
       <c r="E20" s="12" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -4817,7 +4889,7 @@
         <v/>
       </c>
       <c r="T20" s="12" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="U20" s="12" t="str">
@@ -4830,12 +4902,12 @@
       </c>
       <c r="W20" s="12" t="str">
         <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="X20" s="12" t="str">
+        <f t="shared" si="2"/>
         <v>☆</v>
       </c>
-      <c r="X20" s="12" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
       <c r="Y20" s="12" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -4876,21 +4948,24 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-    </row>
-    <row r="21" spans="1:34" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="10" t="s">
+      <c r="AI20" s="12" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="21" spans="1:35" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A21" s="25">
+        <v>8</v>
+      </c>
+      <c r="B21" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="B21" s="11">
+      <c r="C21" s="11">
         <v>2</v>
       </c>
-      <c r="C21" s="5">
+      <c r="D21" s="5">
         <v>45098</v>
       </c>
-      <c r="D21" s="12" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
       <c r="E21" s="12" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -4952,7 +5027,7 @@
         <v/>
       </c>
       <c r="T21" s="12" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="U21" s="12" t="str">
@@ -4969,12 +5044,12 @@
       </c>
       <c r="X21" s="12" t="str">
         <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="Y21" s="12" t="str">
+        <f t="shared" si="2"/>
         <v>☆</v>
       </c>
-      <c r="Y21" s="12" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
       <c r="Z21" s="12" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -5011,21 +5086,24 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-    </row>
-    <row r="22" spans="1:34" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A22" s="10" t="s">
+      <c r="AI21" s="12" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="22" spans="1:35" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A22" s="25">
+        <v>6</v>
+      </c>
+      <c r="B22" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="B22" s="11">
+      <c r="C22" s="11">
         <v>3</v>
       </c>
-      <c r="C22" s="5">
+      <c r="D22" s="5">
         <v>45096</v>
       </c>
-      <c r="D22" s="12" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
       <c r="E22" s="12" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -5087,7 +5165,7 @@
         <v/>
       </c>
       <c r="T22" s="12" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="U22" s="12" t="str">
@@ -5096,12 +5174,12 @@
       </c>
       <c r="V22" s="12" t="str">
         <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="W22" s="12" t="str">
+        <f t="shared" si="2"/>
         <v>☆</v>
       </c>
-      <c r="W22" s="12" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
       <c r="X22" s="12" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -5146,21 +5224,24 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-    </row>
-    <row r="23" spans="1:34" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="10" t="s">
+      <c r="AI22" s="12" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="23" spans="1:35" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A23" s="25">
+        <v>7</v>
+      </c>
+      <c r="B23" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="B23" s="11">
+      <c r="C23" s="11">
         <v>3</v>
       </c>
-      <c r="C23" s="5">
+      <c r="D23" s="5">
         <v>45097</v>
       </c>
-      <c r="D23" s="12" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
       <c r="E23" s="12" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -5222,7 +5303,7 @@
         <v/>
       </c>
       <c r="T23" s="12" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="U23" s="12" t="str">
@@ -5235,12 +5316,12 @@
       </c>
       <c r="W23" s="12" t="str">
         <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="X23" s="12" t="str">
+        <f t="shared" si="2"/>
         <v>☆</v>
       </c>
-      <c r="X23" s="12" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
       <c r="Y23" s="12" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -5281,21 +5362,24 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-    </row>
-    <row r="24" spans="1:34" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A24" s="10" t="s">
+      <c r="AI23" s="12" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="24" spans="1:35" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A24" s="25">
+        <v>8</v>
+      </c>
+      <c r="B24" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="B24" s="11">
+      <c r="C24" s="11">
         <v>3</v>
       </c>
-      <c r="C24" s="5">
+      <c r="D24" s="5">
         <v>45098</v>
       </c>
-      <c r="D24" s="12" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
       <c r="E24" s="12" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -5357,7 +5441,7 @@
         <v/>
       </c>
       <c r="T24" s="12" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="U24" s="12" t="str">
@@ -5374,12 +5458,12 @@
       </c>
       <c r="X24" s="12" t="str">
         <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="Y24" s="12" t="str">
+        <f t="shared" si="2"/>
         <v>☆</v>
       </c>
-      <c r="Y24" s="12" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
       <c r="Z24" s="12" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -5416,21 +5500,24 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-    </row>
-    <row r="25" spans="1:34" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A25" s="10" t="s">
+      <c r="AI24" s="12" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="25" spans="1:35" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A25" s="25">
+        <v>9</v>
+      </c>
+      <c r="B25" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B25" s="11">
+      <c r="C25" s="11">
         <v>1</v>
       </c>
-      <c r="C25" s="5">
+      <c r="D25" s="5">
         <v>45092</v>
       </c>
-      <c r="D25" s="12" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
       <c r="E25" s="12" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -5485,14 +5572,14 @@
       </c>
       <c r="R25" s="12" t="str">
         <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="S25" s="12" t="str">
+        <f t="shared" si="1"/>
         <v>☆</v>
       </c>
-      <c r="S25" s="12" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
       <c r="T25" s="12" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="U25" s="12" t="str">
@@ -5551,21 +5638,24 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-    </row>
-    <row r="26" spans="1:34" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A26" s="10" t="s">
+      <c r="AI25" s="12" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="26" spans="1:35" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A26" s="25">
+        <v>9</v>
+      </c>
+      <c r="B26" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B26" s="11">
+      <c r="C26" s="11">
         <v>2</v>
       </c>
-      <c r="C26" s="5">
+      <c r="D26" s="5">
         <v>45092</v>
       </c>
-      <c r="D26" s="12" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
       <c r="E26" s="12" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -5591,11 +5681,11 @@
         <v/>
       </c>
       <c r="K26" s="12" t="str">
-        <f t="shared" ref="K26:Z53" si="3">IF($C26=K$1,"☆","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="L26" s="12" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="L26:AA27" si="3">IF($D26=L$1,"☆","")</f>
         <v/>
       </c>
       <c r="M26" s="12" t="str">
@@ -5620,11 +5710,11 @@
       </c>
       <c r="R26" s="12" t="str">
         <f t="shared" si="3"/>
-        <v>☆</v>
+        <v/>
       </c>
       <c r="S26" s="12" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>☆</v>
       </c>
       <c r="T26" s="12" t="str">
         <f t="shared" si="3"/>
@@ -5655,7 +5745,7 @@
         <v/>
       </c>
       <c r="AA26" s="12" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="AB26" s="12" t="str">
@@ -5686,23 +5776,26 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-    </row>
-    <row r="27" spans="1:34" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A27" s="10" t="s">
+      <c r="AI26" s="12" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="27" spans="1:35" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A27" s="25">
+        <v>9</v>
+      </c>
+      <c r="B27" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B27" s="11">
+      <c r="C27" s="11">
         <v>3</v>
       </c>
-      <c r="C27" s="5">
+      <c r="D27" s="5">
         <v>45092</v>
       </c>
-      <c r="D27" s="12" t="str">
-        <f t="shared" ref="D27:S53" si="4">IF($C27=D$1,"☆","")</f>
-        <v/>
-      </c>
       <c r="E27" s="12" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="E27:T51" si="4">IF($D27=E$1,"☆","")</f>
         <v/>
       </c>
       <c r="F27" s="12" t="str">
@@ -5755,14 +5848,14 @@
       </c>
       <c r="R27" s="12" t="str">
         <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="S27" s="12" t="str">
+        <f t="shared" si="4"/>
         <v>☆</v>
       </c>
-      <c r="S27" s="12" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
       <c r="T27" s="12" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="U27" s="12" t="str">
@@ -5790,7 +5883,7 @@
         <v/>
       </c>
       <c r="AA27" s="12" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="AB27" s="12" t="str">
@@ -5818,26 +5911,29 @@
         <v/>
       </c>
       <c r="AH27" s="12" t="str">
-        <f t="shared" ref="E27:AH53" si="5">IF($C27=AH$1,"☆","")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="28" spans="1:34" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A28" s="10" t="s">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="AI27" s="12" t="str">
+        <f t="shared" ref="F27:AI36" si="5">IF($D27=AI$1,"☆","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="28" spans="1:35" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A28" s="25">
+        <v>9</v>
+      </c>
+      <c r="B28" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B28" s="11">
+      <c r="C28" s="11">
         <v>4</v>
       </c>
-      <c r="C28" s="5">
+      <c r="D28" s="5">
         <v>45092</v>
       </c>
-      <c r="D28" s="12" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
       <c r="E28" s="12" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="F28" s="12" t="str">
@@ -5890,12 +5986,12 @@
       </c>
       <c r="R28" s="12" t="str">
         <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="S28" s="12" t="str">
+        <f t="shared" si="5"/>
         <v>☆</v>
       </c>
-      <c r="S28" s="12" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
       <c r="T28" s="12" t="str">
         <f t="shared" si="5"/>
         <v/>
@@ -5956,23 +6052,26 @@
         <f t="shared" si="5"/>
         <v/>
       </c>
-    </row>
-    <row r="29" spans="1:34" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A29" s="10" t="s">
+      <c r="AI28" s="12" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+    </row>
+    <row r="29" spans="1:35" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A29" s="25">
+        <v>10</v>
+      </c>
+      <c r="B29" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B29" s="11">
+      <c r="C29" s="11">
         <v>1</v>
       </c>
-      <c r="C29" s="5">
+      <c r="D29" s="5">
         <v>45096</v>
       </c>
-      <c r="D29" s="12" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
       <c r="E29" s="12" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="F29" s="12" t="str">
@@ -6041,12 +6140,12 @@
       </c>
       <c r="V29" s="12" t="str">
         <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="W29" s="12" t="str">
+        <f t="shared" si="5"/>
         <v>☆</v>
       </c>
-      <c r="W29" s="12" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
       <c r="X29" s="12" t="str">
         <f t="shared" si="5"/>
         <v/>
@@ -6091,23 +6190,26 @@
         <f t="shared" si="5"/>
         <v/>
       </c>
-    </row>
-    <row r="30" spans="1:34" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A30" s="10" t="s">
+      <c r="AI29" s="12" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+    </row>
+    <row r="30" spans="1:35" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A30" s="25">
+        <v>10</v>
+      </c>
+      <c r="B30" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B30" s="11">
+      <c r="C30" s="11">
         <v>2</v>
       </c>
-      <c r="C30" s="5">
+      <c r="D30" s="5">
         <v>45096</v>
       </c>
-      <c r="D30" s="12" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
       <c r="E30" s="12" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="F30" s="12" t="str">
@@ -6176,12 +6278,12 @@
       </c>
       <c r="V30" s="12" t="str">
         <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="W30" s="12" t="str">
+        <f t="shared" si="5"/>
         <v>☆</v>
       </c>
-      <c r="W30" s="12" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
       <c r="X30" s="12" t="str">
         <f t="shared" si="5"/>
         <v/>
@@ -6226,23 +6328,26 @@
         <f t="shared" si="5"/>
         <v/>
       </c>
-    </row>
-    <row r="31" spans="1:34" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A31" s="10" t="s">
+      <c r="AI30" s="12" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+    </row>
+    <row r="31" spans="1:35" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A31" s="25">
+        <v>11</v>
+      </c>
+      <c r="B31" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B31" s="11">
+      <c r="C31" s="11">
         <v>1</v>
       </c>
-      <c r="C31" s="5">
+      <c r="D31" s="5">
         <v>45089</v>
       </c>
-      <c r="D31" s="12" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
       <c r="E31" s="12" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="F31" s="12" t="str">
@@ -6283,12 +6388,12 @@
       </c>
       <c r="O31" s="12" t="str">
         <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="P31" s="12" t="str">
+        <f t="shared" si="5"/>
         <v>☆</v>
       </c>
-      <c r="P31" s="12" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
       <c r="Q31" s="12" t="str">
         <f t="shared" si="5"/>
         <v/>
@@ -6361,23 +6466,26 @@
         <f t="shared" si="5"/>
         <v/>
       </c>
-    </row>
-    <row r="32" spans="1:34" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A32" s="10" t="s">
+      <c r="AI31" s="12" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+    </row>
+    <row r="32" spans="1:35" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A32" s="25">
+        <v>11</v>
+      </c>
+      <c r="B32" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B32" s="11">
+      <c r="C32" s="11">
         <v>2</v>
       </c>
-      <c r="C32" s="5">
+      <c r="D32" s="5">
         <v>45089</v>
       </c>
-      <c r="D32" s="12" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
       <c r="E32" s="12" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="F32" s="12" t="str">
@@ -6418,12 +6526,12 @@
       </c>
       <c r="O32" s="12" t="str">
         <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="P32" s="12" t="str">
+        <f t="shared" si="5"/>
         <v>☆</v>
       </c>
-      <c r="P32" s="12" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
       <c r="Q32" s="12" t="str">
         <f t="shared" si="5"/>
         <v/>
@@ -6496,23 +6604,26 @@
         <f t="shared" si="5"/>
         <v/>
       </c>
-    </row>
-    <row r="33" spans="1:34" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A33" s="10" t="s">
+      <c r="AI32" s="12" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+    </row>
+    <row r="33" spans="1:35" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A33" s="25">
+        <v>11</v>
+      </c>
+      <c r="B33" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B33" s="11">
+      <c r="C33" s="11">
         <v>3</v>
       </c>
-      <c r="C33" s="5">
+      <c r="D33" s="5">
         <v>45089</v>
       </c>
-      <c r="D33" s="12" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
       <c r="E33" s="12" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="F33" s="12" t="str">
@@ -6553,12 +6664,12 @@
       </c>
       <c r="O33" s="12" t="str">
         <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="P33" s="12" t="str">
+        <f t="shared" si="5"/>
         <v>☆</v>
       </c>
-      <c r="P33" s="12" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
       <c r="Q33" s="12" t="str">
         <f t="shared" si="5"/>
         <v/>
@@ -6631,23 +6742,26 @@
         <f t="shared" si="5"/>
         <v/>
       </c>
-    </row>
-    <row r="34" spans="1:34" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A34" s="10" t="s">
+      <c r="AI33" s="12" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+    </row>
+    <row r="34" spans="1:35" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A34" s="25">
+        <v>12</v>
+      </c>
+      <c r="B34" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="B34" s="11">
+      <c r="C34" s="11">
         <v>1</v>
       </c>
-      <c r="C34" s="5">
+      <c r="D34" s="5">
         <v>45099</v>
       </c>
-      <c r="D34" s="12" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
       <c r="E34" s="12" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="F34" s="12" t="str">
@@ -6728,12 +6842,12 @@
       </c>
       <c r="Y34" s="12" t="str">
         <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="Z34" s="12" t="str">
+        <f t="shared" si="5"/>
         <v>☆</v>
       </c>
-      <c r="Z34" s="12" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
       <c r="AA34" s="12" t="str">
         <f t="shared" si="5"/>
         <v/>
@@ -6766,23 +6880,26 @@
         <f t="shared" si="5"/>
         <v/>
       </c>
-    </row>
-    <row r="35" spans="1:34" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A35" s="10" t="s">
+      <c r="AI34" s="12" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+    </row>
+    <row r="35" spans="1:35" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A35" s="25">
+        <v>13</v>
+      </c>
+      <c r="B35" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="B35" s="11">
+      <c r="C35" s="11">
         <v>1</v>
       </c>
-      <c r="C35" s="5">
+      <c r="D35" s="5">
         <v>45099</v>
       </c>
-      <c r="D35" s="12" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
       <c r="E35" s="12" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="F35" s="12" t="str">
@@ -6863,12 +6980,12 @@
       </c>
       <c r="Y35" s="12" t="str">
         <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="Z35" s="12" t="str">
+        <f t="shared" si="5"/>
         <v>☆</v>
       </c>
-      <c r="Z35" s="12" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
       <c r="AA35" s="12" t="str">
         <f t="shared" si="5"/>
         <v/>
@@ -6901,23 +7018,26 @@
         <f t="shared" si="5"/>
         <v/>
       </c>
-    </row>
-    <row r="36" spans="1:34" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A36" s="10" t="s">
+      <c r="AI35" s="12" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+    </row>
+    <row r="36" spans="1:35" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A36" s="25">
+        <v>13</v>
+      </c>
+      <c r="B36" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="B36" s="11">
+      <c r="C36" s="11">
         <v>2</v>
       </c>
-      <c r="C36" s="5">
+      <c r="D36" s="5">
         <v>45099</v>
       </c>
-      <c r="D36" s="12" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
       <c r="E36" s="12" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="F36" s="12" t="str">
@@ -6973,11 +7093,11 @@
         <v/>
       </c>
       <c r="S36" s="12" t="str">
-        <f t="shared" ref="S36:AH53" si="6">IF($C36=S$1,"☆","")</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="T36" s="12" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" ref="T36:AI53" si="6">IF($D36=T$1,"☆","")</f>
         <v/>
       </c>
       <c r="U36" s="12" t="str">
@@ -6998,12 +7118,12 @@
       </c>
       <c r="Y36" s="12" t="str">
         <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="Z36" s="12" t="str">
+        <f t="shared" si="6"/>
         <v>☆</v>
       </c>
-      <c r="Z36" s="12" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
       <c r="AA36" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -7036,21 +7156,24 @@
         <f t="shared" si="6"/>
         <v/>
       </c>
-    </row>
-    <row r="37" spans="1:34" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A37" s="10" t="s">
+      <c r="AI36" s="12" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+    </row>
+    <row r="37" spans="1:35" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A37" s="25">
+        <v>13</v>
+      </c>
+      <c r="B37" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="B37" s="11">
+      <c r="C37" s="11">
         <v>3</v>
       </c>
-      <c r="C37" s="5">
+      <c r="D37" s="5">
         <v>45099</v>
       </c>
-      <c r="D37" s="12" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
       <c r="E37" s="12" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -7112,7 +7235,7 @@
         <v/>
       </c>
       <c r="T37" s="12" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="U37" s="12" t="str">
@@ -7133,12 +7256,12 @@
       </c>
       <c r="Y37" s="12" t="str">
         <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="Z37" s="12" t="str">
+        <f t="shared" si="6"/>
         <v>☆</v>
       </c>
-      <c r="Z37" s="12" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
       <c r="AA37" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -7171,21 +7294,24 @@
         <f t="shared" si="6"/>
         <v/>
       </c>
-    </row>
-    <row r="38" spans="1:34" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A38" s="10" t="s">
+      <c r="AI37" s="12" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+    </row>
+    <row r="38" spans="1:35" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A38" s="25">
+        <v>14</v>
+      </c>
+      <c r="B38" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B38" s="11">
+      <c r="C38" s="11">
         <v>1</v>
       </c>
-      <c r="C38" s="5">
+      <c r="D38" s="5">
         <v>45089</v>
       </c>
-      <c r="D38" s="12" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
       <c r="E38" s="12" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -7228,12 +7354,12 @@
       </c>
       <c r="O38" s="12" t="str">
         <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="P38" s="12" t="str">
+        <f t="shared" si="4"/>
         <v>☆</v>
       </c>
-      <c r="P38" s="12" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
       <c r="Q38" s="12" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -7247,7 +7373,7 @@
         <v/>
       </c>
       <c r="T38" s="12" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="U38" s="12" t="str">
@@ -7306,21 +7432,24 @@
         <f t="shared" si="6"/>
         <v/>
       </c>
-    </row>
-    <row r="39" spans="1:34" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A39" s="10" t="s">
+      <c r="AI38" s="12" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+    </row>
+    <row r="39" spans="1:35" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A39" s="25">
+        <v>15</v>
+      </c>
+      <c r="B39" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="B39" s="11">
+      <c r="C39" s="11">
         <v>1</v>
       </c>
-      <c r="C39" s="5">
+      <c r="D39" s="5">
         <v>45084</v>
       </c>
-      <c r="D39" s="12" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
       <c r="E39" s="12" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -7343,12 +7472,12 @@
       </c>
       <c r="J39" s="12" t="str">
         <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="K39" s="12" t="str">
+        <f t="shared" si="4"/>
         <v>☆</v>
       </c>
-      <c r="K39" s="12" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
       <c r="L39" s="12" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -7382,7 +7511,7 @@
         <v/>
       </c>
       <c r="T39" s="12" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="U39" s="12" t="str">
@@ -7441,21 +7570,24 @@
         <f t="shared" si="6"/>
         <v/>
       </c>
-    </row>
-    <row r="40" spans="1:34" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A40" s="10" t="s">
+      <c r="AI39" s="12" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+    </row>
+    <row r="40" spans="1:35" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A40" s="25">
+        <v>15</v>
+      </c>
+      <c r="B40" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="B40" s="11">
+      <c r="C40" s="11">
         <v>2</v>
       </c>
-      <c r="C40" s="5">
+      <c r="D40" s="5">
         <v>45084</v>
       </c>
-      <c r="D40" s="12" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
       <c r="E40" s="12" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -7478,12 +7610,12 @@
       </c>
       <c r="J40" s="12" t="str">
         <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="K40" s="12" t="str">
+        <f t="shared" si="4"/>
         <v>☆</v>
       </c>
-      <c r="K40" s="12" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
       <c r="L40" s="12" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -7517,7 +7649,7 @@
         <v/>
       </c>
       <c r="T40" s="12" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="U40" s="12" t="str">
@@ -7576,21 +7708,24 @@
         <f t="shared" si="6"/>
         <v/>
       </c>
-    </row>
-    <row r="41" spans="1:34" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A41" s="10" t="s">
+      <c r="AI40" s="12" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+    </row>
+    <row r="41" spans="1:35" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A41" s="25">
+        <v>15</v>
+      </c>
+      <c r="B41" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="B41" s="11">
+      <c r="C41" s="11">
         <v>3</v>
       </c>
-      <c r="C41" s="5">
+      <c r="D41" s="5">
         <v>45084</v>
       </c>
-      <c r="D41" s="12" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
       <c r="E41" s="12" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -7613,12 +7748,12 @@
       </c>
       <c r="J41" s="12" t="str">
         <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="K41" s="12" t="str">
+        <f t="shared" si="4"/>
         <v>☆</v>
       </c>
-      <c r="K41" s="12" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
       <c r="L41" s="12" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -7652,7 +7787,7 @@
         <v/>
       </c>
       <c r="T41" s="12" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="U41" s="12" t="str">
@@ -7711,21 +7846,24 @@
         <f t="shared" si="6"/>
         <v/>
       </c>
-    </row>
-    <row r="42" spans="1:34" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A42" s="10" t="s">
+      <c r="AI41" s="12" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+    </row>
+    <row r="42" spans="1:35" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A42" s="25">
+        <v>16</v>
+      </c>
+      <c r="B42" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="B42" s="11">
+      <c r="C42" s="11">
         <v>1</v>
       </c>
-      <c r="C42" s="5">
+      <c r="D42" s="5">
         <v>45093</v>
       </c>
-      <c r="D42" s="12" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
       <c r="E42" s="12" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -7784,12 +7922,12 @@
       </c>
       <c r="S42" s="12" t="str">
         <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="T42" s="12" t="str">
+        <f t="shared" si="4"/>
         <v>☆</v>
       </c>
-      <c r="T42" s="12" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
       <c r="U42" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -7846,21 +7984,24 @@
         <f t="shared" si="6"/>
         <v/>
       </c>
-    </row>
-    <row r="43" spans="1:34" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A43" s="10" t="s">
+      <c r="AI42" s="12" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+    </row>
+    <row r="43" spans="1:35" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A43" s="25">
+        <v>16</v>
+      </c>
+      <c r="B43" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="B43" s="11">
+      <c r="C43" s="11">
         <v>2</v>
       </c>
-      <c r="C43" s="5">
+      <c r="D43" s="5">
         <v>45093</v>
       </c>
-      <c r="D43" s="12" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
       <c r="E43" s="12" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -7919,12 +8060,12 @@
       </c>
       <c r="S43" s="12" t="str">
         <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="T43" s="12" t="str">
+        <f t="shared" si="4"/>
         <v>☆</v>
       </c>
-      <c r="T43" s="12" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
       <c r="U43" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -7981,21 +8122,24 @@
         <f t="shared" si="6"/>
         <v/>
       </c>
-    </row>
-    <row r="44" spans="1:34" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A44" s="10" t="s">
+      <c r="AI43" s="12" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+    </row>
+    <row r="44" spans="1:35" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A44" s="25">
+        <v>17</v>
+      </c>
+      <c r="B44" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="B44" s="11">
+      <c r="C44" s="11">
         <v>1</v>
       </c>
-      <c r="C44" s="5">
+      <c r="D44" s="5">
         <v>45089</v>
       </c>
-      <c r="D44" s="12" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
       <c r="E44" s="12" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -8038,12 +8182,12 @@
       </c>
       <c r="O44" s="12" t="str">
         <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="P44" s="12" t="str">
+        <f t="shared" si="4"/>
         <v>☆</v>
       </c>
-      <c r="P44" s="12" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
       <c r="Q44" s="12" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -8057,7 +8201,7 @@
         <v/>
       </c>
       <c r="T44" s="12" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="U44" s="12" t="str">
@@ -8116,21 +8260,24 @@
         <f t="shared" si="6"/>
         <v/>
       </c>
-    </row>
-    <row r="45" spans="1:34" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A45" s="10" t="s">
+      <c r="AI44" s="12" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+    </row>
+    <row r="45" spans="1:35" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A45" s="25">
+        <v>17</v>
+      </c>
+      <c r="B45" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="B45" s="11">
+      <c r="C45" s="11">
         <v>2</v>
       </c>
-      <c r="C45" s="5">
+      <c r="D45" s="5">
         <v>45089</v>
       </c>
-      <c r="D45" s="12" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
       <c r="E45" s="12" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -8173,12 +8320,12 @@
       </c>
       <c r="O45" s="12" t="str">
         <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="P45" s="12" t="str">
+        <f t="shared" si="4"/>
         <v>☆</v>
       </c>
-      <c r="P45" s="12" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
       <c r="Q45" s="12" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -8192,7 +8339,7 @@
         <v/>
       </c>
       <c r="T45" s="12" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="U45" s="12" t="str">
@@ -8251,21 +8398,24 @@
         <f t="shared" si="6"/>
         <v/>
       </c>
-    </row>
-    <row r="46" spans="1:34" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A46" s="10" t="s">
+      <c r="AI45" s="12" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+    </row>
+    <row r="46" spans="1:35" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A46" s="25">
+        <v>17</v>
+      </c>
+      <c r="B46" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="B46" s="11">
+      <c r="C46" s="11">
         <v>3</v>
       </c>
-      <c r="C46" s="5">
+      <c r="D46" s="5">
         <v>45089</v>
       </c>
-      <c r="D46" s="12" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
       <c r="E46" s="12" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -8308,12 +8458,12 @@
       </c>
       <c r="O46" s="12" t="str">
         <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="P46" s="12" t="str">
+        <f t="shared" si="4"/>
         <v>☆</v>
       </c>
-      <c r="P46" s="12" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
       <c r="Q46" s="12" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -8327,7 +8477,7 @@
         <v/>
       </c>
       <c r="T46" s="12" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="U46" s="12" t="str">
@@ -8386,21 +8536,24 @@
         <f t="shared" si="6"/>
         <v/>
       </c>
-    </row>
-    <row r="47" spans="1:34" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A47" s="10" t="s">
+      <c r="AI46" s="12" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+    </row>
+    <row r="47" spans="1:35" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A47" s="25">
+        <v>18</v>
+      </c>
+      <c r="B47" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="B47" s="11">
+      <c r="C47" s="11">
         <v>1</v>
       </c>
-      <c r="C47" s="5">
+      <c r="D47" s="5">
         <v>45089</v>
       </c>
-      <c r="D47" s="12" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
       <c r="E47" s="12" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -8443,12 +8596,12 @@
       </c>
       <c r="O47" s="12" t="str">
         <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="P47" s="12" t="str">
+        <f t="shared" si="4"/>
         <v>☆</v>
       </c>
-      <c r="P47" s="12" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
       <c r="Q47" s="12" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -8462,7 +8615,7 @@
         <v/>
       </c>
       <c r="T47" s="12" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="U47" s="12" t="str">
@@ -8521,21 +8674,24 @@
         <f t="shared" si="6"/>
         <v/>
       </c>
-    </row>
-    <row r="48" spans="1:34" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A48" s="10" t="s">
+      <c r="AI47" s="12" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+    </row>
+    <row r="48" spans="1:35" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A48" s="25">
+        <v>18</v>
+      </c>
+      <c r="B48" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="B48" s="11">
+      <c r="C48" s="11">
         <v>2</v>
       </c>
-      <c r="C48" s="5">
+      <c r="D48" s="5">
         <v>45089</v>
       </c>
-      <c r="D48" s="12" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
       <c r="E48" s="12" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -8578,12 +8734,12 @@
       </c>
       <c r="O48" s="12" t="str">
         <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="P48" s="12" t="str">
+        <f t="shared" si="4"/>
         <v>☆</v>
       </c>
-      <c r="P48" s="12" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
       <c r="Q48" s="12" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -8597,7 +8753,7 @@
         <v/>
       </c>
       <c r="T48" s="12" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="U48" s="12" t="str">
@@ -8656,21 +8812,24 @@
         <f t="shared" si="6"/>
         <v/>
       </c>
-    </row>
-    <row r="49" spans="1:34" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A49" s="10" t="s">
+      <c r="AI48" s="12" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+    </row>
+    <row r="49" spans="1:35" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A49" s="25">
+        <v>18</v>
+      </c>
+      <c r="B49" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="B49" s="11">
+      <c r="C49" s="11">
         <v>3</v>
       </c>
-      <c r="C49" s="5">
+      <c r="D49" s="5">
         <v>45089</v>
       </c>
-      <c r="D49" s="12" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
       <c r="E49" s="12" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -8713,12 +8872,12 @@
       </c>
       <c r="O49" s="12" t="str">
         <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="P49" s="12" t="str">
+        <f t="shared" si="4"/>
         <v>☆</v>
       </c>
-      <c r="P49" s="12" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
       <c r="Q49" s="12" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -8732,7 +8891,7 @@
         <v/>
       </c>
       <c r="T49" s="12" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="U49" s="12" t="str">
@@ -8791,21 +8950,24 @@
         <f t="shared" si="6"/>
         <v/>
       </c>
-    </row>
-    <row r="50" spans="1:34" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A50" s="10" t="s">
+      <c r="AI49" s="12" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+    </row>
+    <row r="50" spans="1:35" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A50" s="25">
+        <v>19</v>
+      </c>
+      <c r="B50" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="B50" s="11">
+      <c r="C50" s="11">
         <v>1</v>
       </c>
-      <c r="C50" s="5">
+      <c r="D50" s="5">
         <v>45089</v>
       </c>
-      <c r="D50" s="12" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
       <c r="E50" s="12" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -8848,12 +9010,12 @@
       </c>
       <c r="O50" s="12" t="str">
         <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="P50" s="12" t="str">
+        <f t="shared" si="4"/>
         <v>☆</v>
       </c>
-      <c r="P50" s="12" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
       <c r="Q50" s="12" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -8867,7 +9029,7 @@
         <v/>
       </c>
       <c r="T50" s="12" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="U50" s="12" t="str">
@@ -8926,21 +9088,24 @@
         <f t="shared" si="6"/>
         <v/>
       </c>
-    </row>
-    <row r="51" spans="1:34" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A51" s="10" t="s">
+      <c r="AI50" s="12" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+    </row>
+    <row r="51" spans="1:35" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A51" s="25">
+        <v>19</v>
+      </c>
+      <c r="B51" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="B51" s="11">
+      <c r="C51" s="11">
         <v>2</v>
       </c>
-      <c r="C51" s="5">
+      <c r="D51" s="5">
         <v>45089</v>
       </c>
-      <c r="D51" s="12" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
       <c r="E51" s="12" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -8962,11 +9127,11 @@
         <v/>
       </c>
       <c r="J51" s="12" t="str">
-        <f t="shared" ref="J51:Y53" si="7">IF($C51=J$1,"☆","")</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="K51" s="12" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" ref="K51:Z53" si="7">IF($D51=K$1,"☆","")</f>
         <v/>
       </c>
       <c r="L51" s="12" t="str">
@@ -8983,11 +9148,11 @@
       </c>
       <c r="O51" s="12" t="str">
         <f t="shared" si="7"/>
-        <v>☆</v>
+        <v/>
       </c>
       <c r="P51" s="12" t="str">
         <f t="shared" si="7"/>
-        <v/>
+        <v>☆</v>
       </c>
       <c r="Q51" s="12" t="str">
         <f t="shared" si="7"/>
@@ -9026,7 +9191,7 @@
         <v/>
       </c>
       <c r="Z51" s="12" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="AA51" s="12" t="str">
@@ -9061,23 +9226,26 @@
         <f t="shared" si="6"/>
         <v/>
       </c>
-    </row>
-    <row r="52" spans="1:34" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A52" s="10" t="s">
+      <c r="AI51" s="12" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+    </row>
+    <row r="52" spans="1:35" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A52" s="25">
+        <v>19</v>
+      </c>
+      <c r="B52" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="B52" s="11">
+      <c r="C52" s="11">
         <v>3</v>
       </c>
-      <c r="C52" s="5">
+      <c r="D52" s="5">
         <v>45089</v>
       </c>
-      <c r="D52" s="12" t="str">
-        <f t="shared" ref="D52:S53" si="8">IF($C52=D$1,"☆","")</f>
-        <v/>
-      </c>
       <c r="E52" s="12" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" ref="E52:T53" si="8">IF($D52=E$1,"☆","")</f>
         <v/>
       </c>
       <c r="F52" s="12" t="str">
@@ -9118,11 +9286,11 @@
       </c>
       <c r="O52" s="12" t="str">
         <f t="shared" si="8"/>
-        <v>☆</v>
+        <v/>
       </c>
       <c r="P52" s="12" t="str">
         <f t="shared" si="8"/>
-        <v/>
+        <v>☆</v>
       </c>
       <c r="Q52" s="12" t="str">
         <f t="shared" si="8"/>
@@ -9137,7 +9305,7 @@
         <v/>
       </c>
       <c r="T52" s="12" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="U52" s="12" t="str">
@@ -9161,7 +9329,7 @@
         <v/>
       </c>
       <c r="Z52" s="12" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="AA52" s="12" t="str">
@@ -9196,20 +9364,23 @@
         <f t="shared" si="6"/>
         <v/>
       </c>
-    </row>
-    <row r="53" spans="1:34" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A53" s="10" t="s">
+      <c r="AI52" s="12" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+    </row>
+    <row r="53" spans="1:35" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A53" s="25">
+        <v>19</v>
+      </c>
+      <c r="B53" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="B53" s="11">
+      <c r="C53" s="11">
         <v>4</v>
       </c>
-      <c r="C53" s="5">
+      <c r="D53" s="5">
         <v>45089</v>
-      </c>
-      <c r="D53" s="12" t="str">
-        <f t="shared" si="8"/>
-        <v/>
       </c>
       <c r="E53" s="12" t="str">
         <f t="shared" si="8"/>
@@ -9253,11 +9424,11 @@
       </c>
       <c r="O53" s="12" t="str">
         <f t="shared" si="8"/>
-        <v>☆</v>
+        <v/>
       </c>
       <c r="P53" s="12" t="str">
         <f t="shared" si="8"/>
-        <v/>
+        <v>☆</v>
       </c>
       <c r="Q53" s="12" t="str">
         <f t="shared" si="8"/>
@@ -9272,7 +9443,7 @@
         <v/>
       </c>
       <c r="T53" s="12" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="U53" s="12" t="str">
@@ -9296,7 +9467,7 @@
         <v/>
       </c>
       <c r="Z53" s="12" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="AA53" s="12" t="str">
@@ -9328,6 +9499,10 @@
         <v/>
       </c>
       <c r="AH53" s="12" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="AI53" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>

</xml_diff>